<commit_message>
Ignore culture when rendering text values
</commit_message>
<xml_diff>
--- a/tools/typographic-scale.xlsx
+++ b/tools/typographic-scale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hbrems/wrk/dev/apps/github/website-astro/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B0986E-E473-D845-A970-2F59C761C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188BE8EB-AEF4-C94B-8BFE-2096A152B0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5F6399DE-E4DA-FC4D-BEC3-57A68BDB327E}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5F6399DE-E4DA-FC4D-BEC3-57A68BDB327E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,10 +165,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -510,28 +509,30 @@
   <dimension ref="B2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:N22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="12" width="17.83203125" customWidth="1"/>
+    <col min="3" max="9" width="17.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="11" max="12" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -541,78 +542,78 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="C9">
         <f>B3*B9</f>
-        <v>28.8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>B3/B6</f>
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f>TEXT(C13,"0.00")</f>
-        <v>15.00</v>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D13" t="str">
+        <f>SUBSTITUTE(TEXT(C13,"0,00"), ",", ".")</f>
+        <v>13.33</v>
       </c>
       <c r="E13" s="1">
         <f>E14/$B$6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F13" s="2" t="str">
-        <f>TEXT(E13,"0.00")</f>
+      <c r="F13" t="str">
+        <f>SUBSTITUTE(TEXT(E13,"0,00"), ",", ".")</f>
         <v>0.83</v>
       </c>
       <c r="G13" s="1">
@@ -621,50 +622,50 @@
       </c>
       <c r="H13">
         <f>$C$9*G13</f>
-        <v>28.8</v>
-      </c>
-      <c r="I13" s="5">
+        <v>24</v>
+      </c>
+      <c r="I13" s="4">
         <f>K13*G13</f>
-        <v>1.9200000000000002</v>
-      </c>
-      <c r="J13" s="5" t="str">
-        <f>TEXT(I13, "0.0000")</f>
-        <v>1.9200</v>
-      </c>
-      <c r="K13" s="5">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="J13" t="str">
+        <f>SUBSTITUTE(TEXT(I13,"0,0000"), ",", ".")</f>
+        <v>1.8000</v>
+      </c>
+      <c r="K13" s="4">
         <f>$C$9/C13</f>
-        <v>1.9200000000000002</v>
-      </c>
-      <c r="L13" s="5" t="str">
-        <f>TEXT(K13, "0.0000")</f>
-        <v>1.9200</v>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="L13" t="str">
+        <f>SUBSTITUTE(TEXT(K13,"0,0000"), ",", ".")</f>
+        <v>1.8000</v>
       </c>
       <c r="M13" t="str">
         <f>_xlfn.CONCAT(B13, " { ", "font-size: ", F13, "em; ", "line-height: ", J13, "em; ", "margin-top: ", L13, "em; ", "margin-bottom: ", L13, "em; ", "}")</f>
-        <v>small { font-size: 0.83em; line-height: 1.9200em; margin-top: 1.9200em; margin-bottom: 1.9200em; }</v>
+        <v>small { font-size: 0.83em; line-height: 1.8000em; margin-top: 1.8000em; margin-bottom: 1.8000em; }</v>
       </c>
       <c r="N13" t="str">
         <f>_xlfn.CONCAT("--app-",B13, "-font-size: ", F13, "em; ","--app-",B13, "-line-height: ", J13, "em; ","--app-",B13, "-margin: ", L13, "em; ")</f>
-        <v xml:space="preserve">--app-small-font-size: 0.83em; --app-small-line-height: 1.9200em; --app-small-margin: 1.9200em; </v>
+        <v xml:space="preserve">--app-small-font-size: 0.83em; --app-small-line-height: 1.8000em; --app-small-margin: 1.8000em; </v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="1">
         <f>$B$3</f>
-        <v>18</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f>TEXT(C14,"0.00")</f>
-        <v>18.00</v>
+        <v>16</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" ref="D14:D22" si="0">SUBSTITUTE(TEXT(C14,"0,00"), ",", ".")</f>
+        <v>16.00</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="str">
-        <f t="shared" ref="F14:F22" si="0">TEXT(E14,"0.00")</f>
+      <c r="F14" t="str">
+        <f t="shared" ref="F14:F22" si="1">SUBSTITUTE(TEXT(E14,"0,00"), ",", ".")</f>
         <v>1.00</v>
       </c>
       <c r="G14" s="1">
@@ -673,51 +674,51 @@
       </c>
       <c r="H14">
         <f>$C$9*G14</f>
-        <v>28.8</v>
-      </c>
-      <c r="I14" s="5">
+        <v>24</v>
+      </c>
+      <c r="I14" s="4">
         <f>K14*G14</f>
-        <v>1.6</v>
-      </c>
-      <c r="J14" s="5" t="str">
-        <f>TEXT(I14, "0.0000")</f>
-        <v>1.6000</v>
-      </c>
-      <c r="K14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ref="J14:J22" si="2">SUBSTITUTE(TEXT(I14,"0,0000"), ",", ".")</f>
+        <v>1.5000</v>
+      </c>
+      <c r="K14" s="4">
         <f>$C$9/C14</f>
-        <v>1.6</v>
-      </c>
-      <c r="L14" s="5" t="str">
-        <f>TEXT(K14, "0.0000")</f>
-        <v>1.6000</v>
+        <v>1.5</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" ref="L14:L22" si="3">SUBSTITUTE(TEXT(K14,"0,0000"), ",", ".")</f>
+        <v>1.5000</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" ref="M14:M22" si="1">_xlfn.CONCAT(B14, " { ", "font-size: ", F14, "em; ", "line-height: ", J14, "em; ", "margin-top: ", L14, "em; ", "margin-bottom: ", L14, "em; ", "}")</f>
-        <v>p { font-size: 1.00em; line-height: 1.6000em; margin-top: 1.6000em; margin-bottom: 1.6000em; }</v>
+        <f>_xlfn.CONCAT(B14, " { ", "font-size: ", F14, "em; ", "line-height: ", J14, "em; ", "margin-top: ", L14, "em; ", "margin-bottom: ", L14, "em; ", "}")</f>
+        <v>p { font-size: 1.00em; line-height: 1.5000em; margin-top: 1.5000em; margin-bottom: 1.5000em; }</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" ref="N14:N22" si="2">_xlfn.CONCAT("--app-",B14, "-font-size: ", F14, "em; ","--app-",B14, "-line-height: ", J14, "em; ","--app-",B14, "-margin: ", L14, "em; ")</f>
-        <v xml:space="preserve">--app-p-font-size: 1.00em; --app-p-line-height: 1.6000em; --app-p-margin: 1.6000em; </v>
+        <f>_xlfn.CONCAT("--app-",B14, "-font-size: ", F14, "em; ","--app-",B14, "-line-height: ", J14, "em; ","--app-",B14, "-margin: ", L14, "em; ")</f>
+        <v xml:space="preserve">--app-p-font-size: 1.00em; --app-p-line-height: 1.5000em; --app-p-margin: 1.5000em; </v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:C22" si="3">C14*$B$6</f>
-        <v>21.599999999999998</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f t="shared" ref="D15:D22" si="4">TEXT(C15,"0.00")</f>
-        <v>21.60</v>
+        <f t="shared" ref="C15:C22" si="4">C14*$B$6</f>
+        <v>19.2</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>19.20</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ref="E15:E22" si="5">E14*$B$6</f>
         <v>1.2</v>
       </c>
-      <c r="F15" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
         <v>1.20</v>
       </c>
       <c r="G15" s="1">
@@ -726,51 +727,51 @@
       </c>
       <c r="H15">
         <f t="shared" ref="H15:H22" si="7">$C$9*G15</f>
-        <v>28.8</v>
-      </c>
-      <c r="I15" s="5">
+        <v>24</v>
+      </c>
+      <c r="I15" s="4">
         <f t="shared" ref="I15:I22" si="8">K15*G15</f>
-        <v>1.3333333333333335</v>
-      </c>
-      <c r="J15" s="5" t="str">
-        <f t="shared" ref="J15:J22" si="9">TEXT(I15, "0.0000")</f>
-        <v>1.3333</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" ref="K15:K22" si="10">$C$9/C15</f>
-        <v>1.3333333333333335</v>
-      </c>
-      <c r="L15" s="5" t="str">
-        <f t="shared" ref="L15:L22" si="11">TEXT(K15, "0.0000")</f>
-        <v>1.3333</v>
+        <v>1.25</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="2"/>
+        <v>1.2500</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ref="K15:K22" si="9">$C$9/C15</f>
+        <v>1.25</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="3"/>
+        <v>1.2500</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v>h6 { font-size: 1.20em; line-height: 1.3333em; margin-top: 1.3333em; margin-bottom: 1.3333em; }</v>
+        <f t="shared" ref="M15:M22" si="10">_xlfn.CONCAT(B15, " { ", "font-size: ", F15, "em; ", "line-height: ", J15, "em; ", "margin-top: ", L15, "em; ", "margin-bottom: ", L15, "em; ", "}")</f>
+        <v>h6 { font-size: 1.20em; line-height: 1.2500em; margin-top: 1.2500em; margin-bottom: 1.2500em; }</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h6-font-size: 1.20em; --app-h6-line-height: 1.3333em; --app-h6-margin: 1.3333em; </v>
+        <f t="shared" ref="N15:N22" si="11">_xlfn.CONCAT("--app-",B15, "-font-size: ", F15, "em; ","--app-",B15, "-line-height: ", J15, "em; ","--app-",B15, "-margin: ", L15, "em; ")</f>
+        <v xml:space="preserve">--app-h6-font-size: 1.20em; --app-h6-line-height: 1.2500em; --app-h6-margin: 1.2500em; </v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="3"/>
-        <v>25.919999999999998</v>
-      </c>
-      <c r="D16" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>25.92</v>
+        <v>23.04</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>23.04</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="5"/>
         <v>1.44</v>
       </c>
-      <c r="F16" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
         <v>1.44</v>
       </c>
       <c r="G16" s="1">
@@ -779,51 +780,51 @@
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
-        <v>28.8</v>
-      </c>
-      <c r="I16" s="5">
+        <v>24</v>
+      </c>
+      <c r="I16" s="4">
         <f t="shared" si="8"/>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="J16" s="5" t="str">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="2"/>
+        <v>1.0417</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="9"/>
-        <v>1.1111</v>
-      </c>
-      <c r="K16" s="5">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="3"/>
+        <v>1.0417</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="10"/>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="L16" s="5" t="str">
+        <v>h5 { font-size: 1.44em; line-height: 1.0417em; margin-top: 1.0417em; margin-bottom: 1.0417em; }</v>
+      </c>
+      <c r="N16" t="str">
         <f t="shared" si="11"/>
-        <v>1.1111</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v>h5 { font-size: 1.44em; line-height: 1.1111em; margin-top: 1.1111em; margin-bottom: 1.1111em; }</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h5-font-size: 1.44em; --app-h5-line-height: 1.1111em; --app-h5-margin: 1.1111em; </v>
+        <v xml:space="preserve">--app-h5-font-size: 1.44em; --app-h5-line-height: 1.0417em; --app-h5-margin: 1.0417em; </v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="3"/>
-        <v>31.103999999999996</v>
-      </c>
-      <c r="D17" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>31.10</v>
+        <v>27.648</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>27.65</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="5"/>
         <v>1.728</v>
       </c>
-      <c r="F17" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
         <v>1.73</v>
       </c>
       <c r="G17" s="1">
@@ -832,51 +833,51 @@
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
-        <v>57.6</v>
-      </c>
-      <c r="I17" s="5">
+        <v>48</v>
+      </c>
+      <c r="I17" s="4">
         <f t="shared" si="8"/>
-        <v>1.8518518518518521</v>
-      </c>
-      <c r="J17" s="5" t="str">
+        <v>1.7361111111111112</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="2"/>
+        <v>1.7361</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="9"/>
-        <v>1.8519</v>
-      </c>
-      <c r="K17" s="5">
+        <v>0.86805555555555558</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="3"/>
+        <v>0.8681</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="10"/>
-        <v>0.92592592592592604</v>
-      </c>
-      <c r="L17" s="5" t="str">
+        <v>h4 { font-size: 1.73em; line-height: 1.7361em; margin-top: 0.8681em; margin-bottom: 0.8681em; }</v>
+      </c>
+      <c r="N17" t="str">
         <f t="shared" si="11"/>
-        <v>0.9259</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v>h4 { font-size: 1.73em; line-height: 1.8519em; margin-top: 0.9259em; margin-bottom: 0.9259em; }</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h4-font-size: 1.73em; --app-h4-line-height: 1.8519em; --app-h4-margin: 0.9259em; </v>
+        <v xml:space="preserve">--app-h4-font-size: 1.73em; --app-h4-line-height: 1.7361em; --app-h4-margin: 0.8681em; </v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="3"/>
-        <v>37.324799999999996</v>
-      </c>
-      <c r="D18" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>37.32</v>
+        <v>33.177599999999998</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>33.18</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="5"/>
         <v>2.0735999999999999</v>
       </c>
-      <c r="F18" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
         <v>2.07</v>
       </c>
       <c r="G18" s="1">
@@ -885,51 +886,51 @@
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
-        <v>57.6</v>
-      </c>
-      <c r="I18" s="5">
+        <v>48</v>
+      </c>
+      <c r="I18" s="4">
         <f t="shared" si="8"/>
-        <v>1.5432098765432101</v>
-      </c>
-      <c r="J18" s="5" t="str">
+        <v>1.4467592592592593</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="2"/>
+        <v>1.4468</v>
+      </c>
+      <c r="K18" s="4">
         <f t="shared" si="9"/>
-        <v>1.5432</v>
-      </c>
-      <c r="K18" s="5">
+        <v>0.72337962962962965</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="3"/>
+        <v>0.7234</v>
+      </c>
+      <c r="M18" t="str">
         <f t="shared" si="10"/>
-        <v>0.77160493827160503</v>
-      </c>
-      <c r="L18" s="5" t="str">
+        <v>h3 { font-size: 2.07em; line-height: 1.4468em; margin-top: 0.7234em; margin-bottom: 0.7234em; }</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="11"/>
-        <v>0.7716</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="1"/>
-        <v>h3 { font-size: 2.07em; line-height: 1.5432em; margin-top: 0.7716em; margin-bottom: 0.7716em; }</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h3-font-size: 2.07em; --app-h3-line-height: 1.5432em; --app-h3-margin: 0.7716em; </v>
+        <v xml:space="preserve">--app-h3-font-size: 2.07em; --app-h3-line-height: 1.4468em; --app-h3-margin: 0.7234em; </v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="3"/>
-        <v>44.789759999999994</v>
-      </c>
-      <c r="D19" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>44.79</v>
+        <v>39.813119999999998</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>39.81</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="5"/>
         <v>2.4883199999999999</v>
       </c>
-      <c r="F19" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
         <v>2.49</v>
       </c>
       <c r="G19" s="1">
@@ -938,51 +939,51 @@
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
-        <v>57.6</v>
-      </c>
-      <c r="I19" s="5">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4">
         <f t="shared" si="8"/>
-        <v>1.2860082304526752</v>
-      </c>
-      <c r="J19" s="5" t="str">
+        <v>1.2056327160493827</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v>1.2056</v>
+      </c>
+      <c r="K19" s="4">
         <f t="shared" si="9"/>
-        <v>1.2860</v>
-      </c>
-      <c r="K19" s="5">
+        <v>0.60281635802469136</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="3"/>
+        <v>0.6028</v>
+      </c>
+      <c r="M19" t="str">
         <f t="shared" si="10"/>
-        <v>0.6430041152263376</v>
-      </c>
-      <c r="L19" s="5" t="str">
+        <v>h2 { font-size: 2.49em; line-height: 1.2056em; margin-top: 0.6028em; margin-bottom: 0.6028em; }</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="11"/>
-        <v>0.6430</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="1"/>
-        <v>h2 { font-size: 2.49em; line-height: 1.2860em; margin-top: 0.6430em; margin-bottom: 0.6430em; }</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h2-font-size: 2.49em; --app-h2-line-height: 1.2860em; --app-h2-margin: 0.6430em; </v>
+        <v xml:space="preserve">--app-h2-font-size: 2.49em; --app-h2-line-height: 1.2056em; --app-h2-margin: 0.6028em; </v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="3"/>
-        <v>53.747711999999993</v>
-      </c>
-      <c r="D20" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>53.75</v>
+        <v>47.775743999999996</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>47.78</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="5"/>
         <v>2.9859839999999997</v>
       </c>
-      <c r="F20" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
         <v>2.99</v>
       </c>
       <c r="G20" s="1">
@@ -991,51 +992,51 @@
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
-        <v>57.6</v>
-      </c>
-      <c r="I20" s="5">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4">
         <f t="shared" si="8"/>
-        <v>1.0716735253772292</v>
-      </c>
-      <c r="J20" s="5" t="str">
+        <v>1.0046939300411524</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="2"/>
+        <v>1.0047</v>
+      </c>
+      <c r="K20" s="4">
         <f t="shared" si="9"/>
-        <v>1.0717</v>
-      </c>
-      <c r="K20" s="5">
+        <v>0.50234696502057619</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="3"/>
+        <v>0.5023</v>
+      </c>
+      <c r="M20" t="str">
         <f t="shared" si="10"/>
-        <v>0.53583676268861458</v>
-      </c>
-      <c r="L20" s="5" t="str">
+        <v>h1 { font-size: 2.99em; line-height: 1.0047em; margin-top: 0.5023em; margin-bottom: 0.5023em; }</v>
+      </c>
+      <c r="N20" t="str">
         <f t="shared" si="11"/>
-        <v>0.5358</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" si="1"/>
-        <v>h1 { font-size: 2.99em; line-height: 1.0717em; margin-top: 0.5358em; margin-bottom: 0.5358em; }</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-h1-font-size: 2.99em; --app-h1-line-height: 1.0717em; --app-h1-margin: 0.5358em; </v>
+        <v xml:space="preserve">--app-h1-font-size: 2.99em; --app-h1-line-height: 1.0047em; --app-h1-margin: 0.5023em; </v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="3"/>
-        <v>64.497254399999989</v>
-      </c>
-      <c r="D21" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>64.50</v>
+        <v>57.330892799999994</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>57.33</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="5"/>
         <v>3.5831807999999996</v>
       </c>
-      <c r="F21" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
         <v>3.58</v>
       </c>
       <c r="G21" s="1">
@@ -1044,51 +1045,51 @@
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
-        <v>86.4</v>
-      </c>
-      <c r="I21" s="5">
+        <v>72</v>
+      </c>
+      <c r="I21" s="4">
         <f t="shared" si="8"/>
-        <v>1.3395919067215365</v>
-      </c>
-      <c r="J21" s="5" t="str">
+        <v>1.2558674125514404</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="2"/>
+        <v>1.2559</v>
+      </c>
+      <c r="K21" s="4">
         <f t="shared" si="9"/>
-        <v>1.3396</v>
-      </c>
-      <c r="K21" s="5">
+        <v>0.41862247085048016</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="3"/>
+        <v>0.4186</v>
+      </c>
+      <c r="M21" t="str">
         <f t="shared" si="10"/>
-        <v>0.44653063557384554</v>
-      </c>
-      <c r="L21" s="5" t="str">
+        <v>xl { font-size: 3.58em; line-height: 1.2559em; margin-top: 0.4186em; margin-bottom: 0.4186em; }</v>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="11"/>
-        <v>0.4465</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="1"/>
-        <v>xl { font-size: 3.58em; line-height: 1.3396em; margin-top: 0.4465em; margin-bottom: 0.4465em; }</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-xl-font-size: 3.58em; --app-xl-line-height: 1.3396em; --app-xl-margin: 0.4465em; </v>
+        <v xml:space="preserve">--app-xl-font-size: 3.58em; --app-xl-line-height: 1.2559em; --app-xl-margin: 0.4186em; </v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="3"/>
-        <v>77.396705279999978</v>
-      </c>
-      <c r="D22" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>77.40</v>
+        <v>68.79707135999999</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>68.80</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="5"/>
         <v>4.2998169599999994</v>
       </c>
-      <c r="F22" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
         <v>4.30</v>
       </c>
       <c r="G22" s="1">
@@ -1097,44 +1098,41 @@
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
-        <v>86.4</v>
-      </c>
-      <c r="I22" s="5">
+        <v>72</v>
+      </c>
+      <c r="I22" s="4">
         <f t="shared" si="8"/>
-        <v>1.1163265889346139</v>
-      </c>
-      <c r="J22" s="5" t="str">
+        <v>1.0465561771262004</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="2"/>
+        <v>1.0466</v>
+      </c>
+      <c r="K22" s="4">
         <f t="shared" si="9"/>
-        <v>1.1163</v>
-      </c>
-      <c r="K22" s="5">
+        <v>0.34885205904206679</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="3"/>
+        <v>0.3489</v>
+      </c>
+      <c r="M22" t="str">
         <f t="shared" si="10"/>
-        <v>0.37210886297820467</v>
-      </c>
-      <c r="L22" s="5" t="str">
+        <v>xxl { font-size: 4.30em; line-height: 1.0466em; margin-top: 0.3489em; margin-bottom: 0.3489em; }</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" si="11"/>
-        <v>0.3721</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" si="1"/>
-        <v>xxl { font-size: 4.30em; line-height: 1.1163em; margin-top: 0.3721em; margin-bottom: 0.3721em; }</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">--app-xxl-font-size: 4.30em; --app-xxl-line-height: 1.1163em; --app-xxl-margin: 0.3721em; </v>
+        <v xml:space="preserve">--app-xxl-font-size: 4.30em; --app-xxl-line-height: 1.0466em; --app-xxl-margin: 0.3489em; </v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,D13:D20)</f>
-        <v>15.00,18.00,21.60,25.92,31.10,37.32,44.79,53.75</v>
+        <v>13.33,16.00,19.20,23.04,27.65,33.18,39.81,47.78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="D15:D22" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>